<commit_message>
Change Backgrounddetection and Data fusion
</commit_message>
<xml_diff>
--- a/Masterarbeit_daten/6.6.4/Gold.xlsx
+++ b/Masterarbeit_daten/6.6.4/Gold.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="11760" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="11760" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
     <sheet name="Partprice" sheetId="5" r:id="rId5"/>
     <sheet name="Inputs" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1333" uniqueCount="571">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1373" uniqueCount="597">
   <si>
     <t>Größensicht</t>
   </si>
@@ -1544,9 +1544,6 @@
     <t>Rest</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t xml:space="preserve">Aluminium (E) </t>
   </si>
   <si>
@@ -1737,6 +1734,87 @@
   </si>
   <si>
     <t>Lotpaste SnAg3.5 PE</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>http://minerals.usgs.gov/minerals/pubs/commodity/aluminum/myb1-2012-alumi.pdf</t>
+  </si>
+  <si>
+    <t>http://minerals.usgs.gov/minerals/pubs/commodity/lead/myb1-2011-lead.pdf</t>
+  </si>
+  <si>
+    <t>Year average</t>
+  </si>
+  <si>
+    <t>Metalname</t>
+  </si>
+  <si>
+    <t>Lead metal</t>
+  </si>
+  <si>
+    <t>Aluminum metal</t>
+  </si>
+  <si>
+    <t>Chromium metal</t>
+  </si>
+  <si>
+    <t>http://minerals.usgs.gov/minerals/pubs/commodity/chromium/myb1-2012-chrom.pdf</t>
+  </si>
+  <si>
+    <t>Cobalt (minimum of 99.8% cobalt)</t>
+  </si>
+  <si>
+    <t>http://minerals.usgs.gov/minerals/pubs/commodity/cobalt/myb1-2012-cobal.pdf</t>
+  </si>
+  <si>
+    <t>http://minerals.usgs.gov/minerals/pubs/commodity/gold/myb1-2011-gold.pdf</t>
+  </si>
+  <si>
+    <t>Gold metal</t>
+  </si>
+  <si>
+    <t>Copper (London Metal Exchange, highgrade)</t>
+  </si>
+  <si>
+    <t>http://minerals.usgs.gov/minerals/pubs/commodity/copper/mcs-2014-coppe.pdf</t>
+  </si>
+  <si>
+    <t>Nickel metal</t>
+  </si>
+  <si>
+    <t>http://minerals.usgs.gov/minerals/pubs/commodity/nickel/myb1-2011-nicke.pdf</t>
+  </si>
+  <si>
+    <t>http://minerals.usgs.gov/minerals/pubs/commodity/platinum/mcs-2014-plati.pdf</t>
+  </si>
+  <si>
+    <t>Palladium metal</t>
+  </si>
+  <si>
+    <t>Platinum metal</t>
+  </si>
+  <si>
+    <t>http://minerals.usgs.gov/minerals/pubs/commodity/silver/myb1-2011-silve.pdf</t>
+  </si>
+  <si>
+    <t>Steal (hot-rolled steel sheet)</t>
+  </si>
+  <si>
+    <t>http://minerals.usgs.gov/minerals/pubs/commodity/iron_&amp;_steel/myb1-2012-feste.pdf</t>
+  </si>
+  <si>
+    <t>Zinc (super high grade (SHG) zinc, 99.995% pure)</t>
+  </si>
+  <si>
+    <t>http://minerals.usgs.gov/minerals/pubs/commodity/zinc/myb1-2012-zinc.pdf</t>
+  </si>
+  <si>
+    <t>http://minerals.usgs.gov/minerals/pubs/commodity/tin/myb1-2012-tin.pdf</t>
+  </si>
+  <si>
+    <t>Tin metal</t>
   </si>
 </sst>
 </file>
@@ -1746,7 +1824,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1769,6 +1847,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1787,10 +1873,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1802,9 +1889,14 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1880,6 +1972,7 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -1902,6 +1995,7 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -1924,6 +2018,7 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -1946,6 +2041,7 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="3"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -1968,6 +2064,7 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="4"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -2060,6 +2157,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -2538,6 +2636,7 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="11"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -2641,67 +2740,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>6.6441207377999998E-4</c:v>
+                  <c:v>6.9605074396000008E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.982574E-6</c:v>
+                  <c:v>2.3790887999999998E-6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.5119999999999999E-8</c:v>
+                  <c:v>3.0143999999999995E-8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.420362E-5</c:v>
+                  <c:v>6.9965979999999999E-5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.2369600000000001E-6</c:v>
+                  <c:v>2.1142880000000003E-6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.85362609840000003</c:v>
+                  <c:v>1.0179491223420001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.0072160000000041</c:v>
+                  <c:v>2.3936050800000048</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.7554030359999997E-2</c:v>
+                  <c:v>4.1537033579999993E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.9627131216000002E-2</c:v>
+                  <c:v>2.1708796648E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.2016660082999999E-3</c:v>
+                  <c:v>1.6882301588999997E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.0215944600000002E-3</c:v>
+                  <c:v>2.8401541799999994E-3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.8128685603999997</c:v>
+                  <c:v>2.2953977407539998</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.8128685603999997</c:v>
+                  <c:v>2.2953977407539998</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.2026152</c:v>
+                  <c:v>0.23000139</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.58725225057599995</c:v>
+                  <c:v>1.12466741826528</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.10402624000000001</c:v>
+                  <c:v>0.19922430720000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>9.0950234000000002E-5</c:v>
+                  <c:v>1.1459729484E-4</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4.1030192250000001E-6</c:v>
+                  <c:v>3.5559499949999999E-6</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3.8601E-4</c:v>
+                  <c:v>3.3454199999999996E-4</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5.5418594000000005E-4</c:v>
+                  <c:v>5.7602578E-4</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.102760884156</c:v>
+                  <c:v>0.10681057417200002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4495,7 +4594,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4505,17 +4604,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF422"/>
   <sheetViews>
-    <sheetView topLeftCell="AC25" workbookViewId="0">
-      <selection activeCell="F41" sqref="A41:XFD41"/>
+    <sheetView topLeftCell="L64" workbookViewId="0">
+      <selection activeCell="Q96" sqref="Q96"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="29.5703125" customWidth="1"/>
     <col min="7" max="7" width="15.140625" customWidth="1"/>
     <col min="8" max="8" width="33.28515625" customWidth="1"/>
     <col min="14" max="14" width="11.42578125" customWidth="1"/>
     <col min="16" max="16" width="39.140625" customWidth="1"/>
+    <col min="19" max="20" width="34.85546875" customWidth="1"/>
     <col min="22" max="22" width="17.42578125" customWidth="1"/>
     <col min="27" max="27" width="33.5703125" customWidth="1"/>
     <col min="28" max="28" width="46.85546875" customWidth="1"/>
@@ -41361,7 +41461,7 @@
       <selection sqref="A1:A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="83.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
@@ -41373,7 +41473,7 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B1">
         <v>0</v>
@@ -41388,7 +41488,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -41403,7 +41503,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B3" s="1">
         <v>-1.664E-5</v>
@@ -41422,7 +41522,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B4" s="1">
         <v>-2.2400000000000002E-6</v>
@@ -41439,7 +41539,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B5" s="1">
         <v>-2.5509100000000002E-7</v>
@@ -41454,7 +41554,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -41469,7 +41569,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -41484,7 +41584,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -41499,7 +41599,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -41514,7 +41614,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -41529,7 +41629,7 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -41544,7 +41644,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -41559,7 +41659,7 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -41574,7 +41674,7 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -41589,7 +41689,7 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -41604,7 +41704,7 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -41619,7 +41719,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -41634,7 +41734,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -41649,7 +41749,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -41697,18 +41797,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:AH42"/>
+  <dimension ref="B1:AH47"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="M54" sqref="M54"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="45.85546875" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.7109375" customWidth="1"/>
     <col min="5" max="5" width="19.28515625" customWidth="1"/>
+    <col min="6" max="6" width="44.28515625" customWidth="1"/>
+    <col min="7" max="7" width="85.42578125" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:34" x14ac:dyDescent="0.25">
@@ -41724,25 +41827,43 @@
       <c r="E1" t="s">
         <v>448</v>
       </c>
+      <c r="F1" t="s">
+        <v>574</v>
+      </c>
+      <c r="G1" t="s">
+        <v>570</v>
+      </c>
+      <c r="H1" t="s">
+        <v>573</v>
+      </c>
     </row>
     <row r="2" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C2">
         <v>3.1638670179999999E-4</v>
       </c>
       <c r="D2">
-        <v>2.1</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E2">
         <f>C2*D2</f>
-        <v>6.6441207377999998E-4</v>
+        <v>6.9605074396000008E-4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>576</v>
+      </c>
+      <c r="G2" t="s">
+        <v>571</v>
+      </c>
+      <c r="H2">
+        <v>2012</v>
       </c>
     </row>
     <row r="3" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C3">
         <v>2.5105142999999998E-3</v>
@@ -41757,7 +41878,7 @@
     </row>
     <row r="4" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C4" s="1">
         <v>1.7401199999999999E-8</v>
@@ -41772,7 +41893,7 @@
     </row>
     <row r="5" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C5" s="1">
         <v>1.4131835999999999E-5</v>
@@ -41787,70 +41908,106 @@
     </row>
     <row r="6" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C6" s="1">
         <v>9.91287E-7</v>
       </c>
       <c r="D6">
-        <v>2</v>
+        <v>2.4</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>1.982574E-6</v>
+        <v>2.3790887999999998E-6</v>
+      </c>
+      <c r="F6" t="s">
+        <v>575</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>572</v>
+      </c>
+      <c r="H6">
+        <v>2011</v>
       </c>
     </row>
     <row r="7" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C7" s="1">
         <v>1.256E-8</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>2.4</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>2.5119999999999999E-8</v>
+        <v>3.0143999999999995E-8</v>
+      </c>
+      <c r="F7" t="s">
+        <v>575</v>
+      </c>
+      <c r="G7" t="s">
+        <v>572</v>
+      </c>
+      <c r="H7">
+        <v>2011</v>
       </c>
     </row>
     <row r="8" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C8" s="1">
         <v>5.2606000000000001E-6</v>
       </c>
       <c r="D8">
-        <v>2.7</v>
+        <v>13.3</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>1.420362E-5</v>
+        <v>6.9965979999999999E-5</v>
+      </c>
+      <c r="F8" t="s">
+        <v>577</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>578</v>
+      </c>
+      <c r="H8">
+        <v>2012</v>
       </c>
     </row>
     <row r="9" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C9" s="1">
         <v>7.2160000000000006E-8</v>
       </c>
       <c r="D9">
-        <v>31</v>
+        <v>29.3</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>2.2369600000000001E-6</v>
+        <v>2.1142880000000003E-6</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>579</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>580</v>
+      </c>
+      <c r="H9">
+        <v>2012</v>
       </c>
       <c r="AH9" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="10" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C10" s="1">
         <v>3.7001800000000002E-5</v>
@@ -41865,7 +42022,7 @@
     </row>
     <row r="11" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C11" s="1">
         <v>6.6000000000000005E-5</v>
@@ -41880,7 +42037,7 @@
     </row>
     <row r="12" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C12">
         <v>5.5667235900000002E-3</v>
@@ -41895,7 +42052,7 @@
     </row>
     <row r="13" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B13" s="6" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C13">
         <v>1.044E-4</v>
@@ -41910,7 +42067,7 @@
     </row>
     <row r="14" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C14">
         <v>5.5944999999999996E-4</v>
@@ -41925,7 +42082,7 @@
     </row>
     <row r="15" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C15" s="1">
         <v>8.4201699999999997E-5</v>
@@ -41940,7 +42097,7 @@
     </row>
     <row r="16" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C16">
         <v>5.3119999999999999E-3</v>
@@ -41953,114 +42110,177 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C17" s="1">
         <v>2.0132691E-5</v>
       </c>
       <c r="D17">
-        <v>42400</v>
+        <v>50562</v>
       </c>
       <c r="E17">
         <f t="shared" si="0"/>
-        <v>0.85362609840000003</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+        <v>1.0179491223420001</v>
+      </c>
+      <c r="F17" t="s">
+        <v>582</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>581</v>
+      </c>
+      <c r="H17">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="6" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="C18" s="1">
         <v>4.7340000000000099E-5</v>
       </c>
       <c r="D18">
-        <v>42400</v>
+        <v>50562</v>
       </c>
       <c r="E18">
         <f t="shared" si="0"/>
-        <v>2.0072160000000041</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+        <v>2.3936050800000048</v>
+      </c>
+      <c r="F18" t="s">
+        <v>582</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>581</v>
+      </c>
+      <c r="H18">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="6" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C19">
         <v>5.6900045999999996E-3</v>
       </c>
       <c r="D19">
-        <v>6.6</v>
+        <v>7.3</v>
       </c>
       <c r="E19">
         <f t="shared" si="0"/>
-        <v>3.7554030359999997E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+        <v>4.1537033579999993E-2</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>583</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>584</v>
+      </c>
+      <c r="H19">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="6" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="C20">
         <v>2.9738077600000002E-3</v>
       </c>
       <c r="D20">
-        <v>6.6</v>
+        <v>7.3</v>
       </c>
       <c r="E20">
         <f t="shared" si="0"/>
-        <v>1.9627131216000002E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+        <v>2.1708796648E-2</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>583</v>
+      </c>
+      <c r="G20" t="s">
+        <v>584</v>
+      </c>
+      <c r="H20">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="6" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C21" s="1">
         <v>7.3721840999999995E-5</v>
       </c>
       <c r="D21">
-        <v>16.3</v>
+        <v>22.9</v>
       </c>
       <c r="E21">
         <f t="shared" si="0"/>
-        <v>1.2016660082999999E-3</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+        <v>1.6882301588999997E-3</v>
+      </c>
+      <c r="F21" t="s">
+        <v>585</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>586</v>
+      </c>
+      <c r="H21">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="6" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="C22">
         <v>1.2402419999999999E-4</v>
       </c>
       <c r="D22">
-        <v>16.3</v>
+        <v>22.9</v>
       </c>
       <c r="E22">
         <f t="shared" si="0"/>
-        <v>2.0215944600000002E-3</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+        <v>2.8401541799999994E-3</v>
+      </c>
+      <c r="F22" t="s">
+        <v>585</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>586</v>
+      </c>
+      <c r="H22">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="6" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C23" s="1">
         <v>9.6995467599999996E-5</v>
       </c>
       <c r="D23">
-        <v>29000</v>
+        <v>23665</v>
       </c>
       <c r="E23">
         <f t="shared" si="0"/>
-        <v>2.8128685603999997</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+        <v>2.2953977407539998</v>
+      </c>
+      <c r="F23" t="s">
+        <v>588</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>587</v>
+      </c>
+      <c r="H23">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C24" s="1">
         <v>2.94E-5</v>
@@ -42073,24 +42293,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="6" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C25" s="1">
         <v>4.7339999999999999E-6</v>
       </c>
       <c r="D25">
-        <v>42800</v>
+        <v>48585</v>
       </c>
       <c r="E25">
         <f t="shared" si="0"/>
-        <v>0.2026152</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+        <v>0.23000139</v>
+      </c>
+      <c r="F25" t="s">
+        <v>589</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>587</v>
+      </c>
+      <c r="H25">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="6" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C26" s="1">
         <v>3.9895799999999998E-5</v>
@@ -42103,9 +42332,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="6" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C27" s="1">
         <v>6.7799999999999995E-5</v>
@@ -42118,9 +42347,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="6" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C28" s="1">
         <v>1.8900199999999999E-5</v>
@@ -42133,9 +42362,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="6" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C29" s="1">
         <v>2.0086000000000001E-6</v>
@@ -42148,39 +42377,51 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="6" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C30">
         <v>9.9198015299999998E-4</v>
       </c>
       <c r="D30">
-        <v>592</v>
+        <v>1133.76</v>
       </c>
       <c r="E30">
         <f t="shared" si="0"/>
-        <v>0.58725225057599995</v>
-      </c>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+        <v>1.12466741826528</v>
+      </c>
+      <c r="G30" s="10" t="s">
+        <v>590</v>
+      </c>
+      <c r="H30">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="6" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="C31">
         <v>1.7572E-4</v>
       </c>
       <c r="D31">
-        <v>592</v>
+        <v>1133.76</v>
       </c>
       <c r="E31">
         <f t="shared" si="0"/>
-        <v>0.10402624000000001</v>
-      </c>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+        <v>0.19922430720000001</v>
+      </c>
+      <c r="G31" s="10" t="s">
+        <v>590</v>
+      </c>
+      <c r="H31">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B32" s="6" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="C32" s="1">
         <v>3.6451422000000002E-5</v>
@@ -42195,7 +42436,7 @@
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="6" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C33">
         <v>2.9213824999999999E-3</v>
@@ -42210,7 +42451,7 @@
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" s="6" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="C34" s="1">
         <v>3.9010400000000002E-5</v>
@@ -42225,25 +42466,31 @@
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="6" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="C35">
         <v>1.81900468E-4</v>
       </c>
       <c r="D35">
-        <v>0.5</v>
+        <v>0.63</v>
       </c>
       <c r="E35">
         <f t="shared" si="0"/>
-        <v>9.0950234000000002E-5</v>
-      </c>
-      <c r="H35" t="s">
-        <v>506</v>
+        <v>1.1459729484E-4</v>
+      </c>
+      <c r="F35" t="s">
+        <v>591</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>592</v>
+      </c>
+      <c r="H35">
+        <v>2012</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" s="6" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C36" s="1">
         <v>5.6941618E-5</v>
@@ -42258,7 +42505,7 @@
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" s="6" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="C37" s="1">
         <v>1.3499999999999999E-5</v>
@@ -42273,74 +42520,131 @@
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B38" s="6" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C38" s="1">
         <v>1.8235641E-6</v>
       </c>
       <c r="D38">
-        <v>2.25</v>
+        <v>1.95</v>
       </c>
       <c r="E38">
         <f t="shared" si="0"/>
-        <v>4.1030192250000001E-6</v>
+        <v>3.5559499949999999E-6</v>
+      </c>
+      <c r="F38" t="s">
+        <v>593</v>
+      </c>
+      <c r="G38" s="10" t="s">
+        <v>594</v>
+      </c>
+      <c r="H38">
+        <v>2012</v>
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B39" s="6" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C39">
         <v>1.7155999999999999E-4</v>
       </c>
       <c r="D39">
-        <v>2.25</v>
+        <v>1.95</v>
       </c>
       <c r="E39">
         <f t="shared" si="0"/>
-        <v>3.8601E-4</v>
+        <v>3.3454199999999996E-4</v>
+      </c>
+      <c r="F39" t="s">
+        <v>593</v>
+      </c>
+      <c r="G39" s="10" t="s">
+        <v>594</v>
+      </c>
+      <c r="H39">
+        <v>2012</v>
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B40" s="6" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C40" s="1">
         <v>2.7299799999999999E-5</v>
       </c>
       <c r="D40">
-        <v>20.3</v>
+        <v>21.1</v>
       </c>
       <c r="E40">
         <f t="shared" si="0"/>
-        <v>5.5418594000000005E-4</v>
+        <v>5.7602578E-4</v>
+      </c>
+      <c r="F40" t="s">
+        <v>596</v>
+      </c>
+      <c r="G40" s="10" t="s">
+        <v>595</v>
+      </c>
+      <c r="H40">
+        <v>2012</v>
       </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B41" s="6" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="C41">
         <v>5.0621125200000002E-3</v>
       </c>
       <c r="D41">
-        <v>20.3</v>
+        <v>21.1</v>
       </c>
       <c r="E41">
         <f t="shared" si="0"/>
-        <v>0.102760884156</v>
+        <v>0.10681057417200002</v>
+      </c>
+      <c r="F41" t="s">
+        <v>596</v>
+      </c>
+      <c r="G41" t="s">
+        <v>595</v>
+      </c>
+      <c r="H41">
+        <v>2012</v>
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E42">
         <f>SUM(E2:E41)</f>
-        <v>6.7324877651173081</v>
-      </c>
+        <v>7.4372291085697793</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B47" s="5"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G17" r:id="rId1"/>
+    <hyperlink ref="G18" r:id="rId2"/>
+    <hyperlink ref="G21" r:id="rId3"/>
+    <hyperlink ref="G22" r:id="rId4"/>
+    <hyperlink ref="G25" r:id="rId5"/>
+    <hyperlink ref="G30" r:id="rId6"/>
+    <hyperlink ref="G31" r:id="rId7"/>
+    <hyperlink ref="G38" r:id="rId8"/>
+    <hyperlink ref="G39" r:id="rId9"/>
+    <hyperlink ref="G6" r:id="rId10"/>
+    <hyperlink ref="G8" r:id="rId11"/>
+    <hyperlink ref="G9" r:id="rId12"/>
+    <hyperlink ref="G19" r:id="rId13"/>
+    <hyperlink ref="G23" r:id="rId14"/>
+    <hyperlink ref="G35" r:id="rId15"/>
+    <hyperlink ref="G40" r:id="rId16"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId17"/>
+  <drawing r:id="rId18"/>
 </worksheet>
 </file>
 
@@ -42348,11 +42652,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="73.140625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="47.140625" bestFit="1" customWidth="1"/>
@@ -42361,7 +42665,7 @@
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B1">
         <v>0</v>
@@ -42373,7 +42677,7 @@
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -42395,7 +42699,7 @@
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -42407,7 +42711,7 @@
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -42419,7 +42723,7 @@
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B5" s="1">
         <v>-1.28576E-8</v>
@@ -42431,7 +42735,7 @@
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -42443,7 +42747,7 @@
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -42455,7 +42759,7 @@
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B8" s="1">
         <v>-1.6199999999999999E-7</v>
@@ -42467,7 +42771,7 @@
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B9" s="1">
         <v>-8.5400000000000002E-5</v>
@@ -42479,7 +42783,7 @@
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -42491,7 +42795,7 @@
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -42503,7 +42807,7 @@
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -42515,7 +42819,7 @@
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -42527,7 +42831,7 @@
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -42539,7 +42843,7 @@
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -42551,7 +42855,7 @@
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -42563,7 +42867,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B17" s="1">
         <v>-1.7977500000000001E-6</v>
@@ -42575,7 +42879,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B18" s="1">
         <v>-5.355E-7</v>
@@ -42587,7 +42891,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B19" s="1">
         <v>-9.0780000000000002E-6</v>
@@ -42616,11 +42920,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D70"/>
   <sheetViews>
-    <sheetView topLeftCell="C34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D65" sqref="D65"/>
+    <sheetView topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="58.85546875" style="3" customWidth="1"/>
     <col min="2" max="2" width="51.85546875" style="4" customWidth="1"/>
@@ -43091,7 +43395,7 @@
     </row>
     <row r="39" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C39" s="5">
         <v>0.2</v>
@@ -43099,7 +43403,7 @@
     </row>
     <row r="40" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C40" s="5">
         <v>0.1</v>
@@ -43107,7 +43411,7 @@
     </row>
     <row r="41" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C41" s="5">
         <v>7</v>
@@ -43115,7 +43419,7 @@
     </row>
     <row r="42" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C42" s="5">
         <v>3.4</v>
@@ -43123,7 +43427,7 @@
     </row>
     <row r="43" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C43" s="5">
         <v>0.43</v>
@@ -43131,7 +43435,7 @@
     </row>
     <row r="44" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C44" s="5">
         <v>0.25</v>
@@ -43139,7 +43443,7 @@
     </row>
     <row r="45" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C45" s="5">
         <v>0.03</v>
@@ -43147,7 +43451,7 @@
     </row>
     <row r="46" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="C46" s="5">
         <v>0.03</v>
@@ -43155,7 +43459,7 @@
     </row>
     <row r="47" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="C47" s="5">
         <v>0.03</v>
@@ -43163,7 +43467,7 @@
     </row>
     <row r="48" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="C48" s="5">
         <v>0.25</v>
@@ -43171,7 +43475,7 @@
     </row>
     <row r="49" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C49" s="5">
         <v>0</v>
@@ -43179,7 +43483,7 @@
     </row>
     <row r="50" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="C50" s="5">
         <v>1.2</v>
@@ -43187,7 +43491,7 @@
     </row>
     <row r="51" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C51" s="5">
         <v>0.3</v>
@@ -43195,7 +43499,7 @@
     </row>
     <row r="52" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C52" s="5">
         <v>0.1</v>
@@ -43203,7 +43507,7 @@
     </row>
     <row r="53" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C53" s="5">
         <v>0.1</v>
@@ -43211,7 +43515,7 @@
     </row>
     <row r="54" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C54" s="5">
         <v>0.3</v>
@@ -43219,7 +43523,7 @@
     </row>
     <row r="55" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C55" s="5">
         <v>0.02</v>
@@ -43227,7 +43531,7 @@
     </row>
     <row r="56" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="C56" s="5">
         <v>1.4999999999999999E-2</v>
@@ -43235,7 +43539,7 @@
     </row>
     <row r="57" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="C57" s="5">
         <v>1.4999999999999999E-2</v>
@@ -43243,7 +43547,7 @@
     </row>
     <row r="58" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C58" s="5">
         <v>0.02</v>
@@ -43251,7 +43555,7 @@
     </row>
     <row r="59" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="C59" s="5">
         <v>0</v>
@@ -43259,7 +43563,7 @@
     </row>
     <row r="60" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="C60" s="5">
         <v>1.2</v>
@@ -43267,7 +43571,7 @@
     </row>
     <row r="61" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C61" s="5">
         <v>0.1</v>
@@ -43275,7 +43579,7 @@
     </row>
     <row r="62" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C62" s="5">
         <v>0.1</v>
@@ -43283,7 +43587,7 @@
     </row>
     <row r="63" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C63" s="5">
         <v>0.4</v>
@@ -43291,7 +43595,7 @@
     </row>
     <row r="64" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C64" s="5">
         <v>0.3</v>
@@ -43299,7 +43603,7 @@
     </row>
     <row r="65" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C65" s="5">
         <v>0.02</v>
@@ -43307,7 +43611,7 @@
     </row>
     <row r="66" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="C66" s="5">
         <v>1.4999999999999999E-2</v>
@@ -43315,7 +43619,7 @@
     </row>
     <row r="67" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="C67" s="5">
         <v>1.4999999999999999E-2</v>
@@ -43323,7 +43627,7 @@
     </row>
     <row r="68" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C68" s="5">
         <v>0.02</v>
@@ -43353,25 +43657,25 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A20"/>
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="75.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
+        <v>567</v>
+      </c>
+      <c r="B1" t="s">
         <v>568</v>
-      </c>
-      <c r="B1" t="s">
-        <v>569</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -43379,7 +43683,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -43387,7 +43691,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -43395,7 +43699,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -43403,7 +43707,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -43411,7 +43715,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -43419,7 +43723,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B8">
         <v>31</v>
@@ -43427,7 +43731,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -43435,7 +43739,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B10">
         <v>7</v>
@@ -43443,7 +43747,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B11">
         <v>6</v>
@@ -43451,7 +43755,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -43459,7 +43763,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -43467,7 +43771,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -43475,7 +43779,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B15">
         <v>7</v>
@@ -43483,7 +43787,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -43491,7 +43795,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B17">
         <v>6</v>
@@ -43499,7 +43803,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B18">
         <v>47</v>
@@ -43507,7 +43811,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B19">
         <v>5</v>
@@ -43515,7 +43819,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B20">
         <v>20</v>

</xml_diff>